<commit_message>
added propellant properties docs and additions to spreadsheets + scaled circuit
</commit_message>
<xml_diff>
--- a/docs/Propellant Properties.xlsx
+++ b/docs/Propellant Properties.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA77AA53-6AC3-1D46-97A5-C71E1EC1EDB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC776364-ADB4-1D42-A756-399C8B0DF3D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16040" xr2:uid="{56F9EF7F-A7A9-4F41-8447-E1767CFEDAA1}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="27640" windowHeight="16040" activeTab="1" xr2:uid="{56F9EF7F-A7A9-4F41-8447-E1767CFEDAA1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Individual" sheetId="1" r:id="rId1"/>
+    <sheet name="Mixture" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="tables" localSheetId="1">Mixture!$D$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Converse Engine</t>
   </si>
@@ -123,6 +127,33 @@
       </rPr>
       <t>3</t>
     </r>
+  </si>
+  <si>
+    <t>Melting Point</t>
+  </si>
+  <si>
+    <t>Boiling Point</t>
+  </si>
+  <si>
+    <t>Hypergolic</t>
+  </si>
+  <si>
+    <t>Mixture Ratio</t>
+  </si>
+  <si>
+    <t>Density Impulse</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Oxidizer - LOX</t>
+  </si>
+  <si>
+    <t>Fuel - Ethanol</t>
+  </si>
+  <si>
+    <t>Specific Impulse (Sea Level)</t>
   </si>
 </sst>
 </file>
@@ -202,17 +233,17 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EB8C75-839A-4149-AB73-8017B47EF239}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,107 +572,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>-218.8</v>
+      </c>
+      <c r="C13">
+        <v>-114.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>-183</v>
+      </c>
+      <c r="C14">
+        <v>78.2</v>
       </c>
     </row>
   </sheetData>
@@ -650,4 +703,75 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBAC4AD-6539-6D4B-A113-327F84D51EF8}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1.29</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7">
+        <v>269</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7">
+        <v>264</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
work on PID feedback control for engine chill task (ecu firmware)
</commit_message>
<xml_diff>
--- a/docs/Propellant Properties.xlsx
+++ b/docs/Propellant Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC776364-ADB4-1D42-A756-399C8B0DF3D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6398211-5904-EA4B-8E7F-3C4F5437E6C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="27640" windowHeight="16040" activeTab="1" xr2:uid="{56F9EF7F-A7A9-4F41-8447-E1767CFEDAA1}"/>
+    <workbookView xWindow="780" yWindow="740" windowWidth="27640" windowHeight="16040" xr2:uid="{56F9EF7F-A7A9-4F41-8447-E1767CFEDAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Converse Engine</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>Specific Impulse (Sea Level)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Standard Range</t>
+  </si>
+  <si>
+    <t>"-114 &lt;&gt; 78"</t>
+  </si>
+  <si>
+    <t>"-218 &lt;&gt; -182.96"</t>
   </si>
 </sst>
 </file>
@@ -558,20 +570,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EB8C75-839A-4149-AB73-8017B47EF239}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -579,7 +591,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -590,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
@@ -598,7 +610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -609,7 +621,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -620,7 +632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -631,7 +643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -642,7 +654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -653,7 +665,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -664,7 +676,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -675,26 +687,46 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B13">
-        <v>-218.8</v>
+        <v>-114</v>
       </c>
       <c r="C13">
-        <v>-114.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>-218.79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14">
-        <v>-183</v>
+        <v>78</v>
       </c>
       <c r="C14">
-        <v>78.2</v>
+        <v>-182.96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBAC4AD-6539-6D4B-A113-327F84D51EF8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>